<commit_message>
more sprites front back
</commit_message>
<xml_diff>
--- a/screenshots/PokemonLegendsCelebi/PokeDex.xlsx
+++ b/screenshots/PokemonLegendsCelebi/PokeDex.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dwg11\PLC_Polished\screenshots\PokemonLegendsCelebi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{238276D7-3887-4FBE-A4EC-01D28DDC7357}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B403B979-2AF2-4BC1-988A-9C1DE4514861}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="1" xr2:uid="{64765D12-A245-44E0-8473-F56FA5BDDDC6}"/>
+    <workbookView xWindow="3430" yWindow="460" windowWidth="21300" windowHeight="14820" activeTab="1" xr2:uid="{64765D12-A245-44E0-8473-F56FA5BDDDC6}"/>
   </bookViews>
   <sheets>
     <sheet name="Dex" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3691" uniqueCount="908">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3824" uniqueCount="921">
   <si>
     <t xml:space="preserve">cyndaquil		</t>
   </si>
@@ -2763,6 +2763,45 @@
   </si>
   <si>
     <t>left</t>
+  </si>
+  <si>
+    <t>I did</t>
+  </si>
+  <si>
+    <t>fokkos92</t>
+  </si>
+  <si>
+    <t>theymadememakethisac</t>
+  </si>
+  <si>
+    <t>fokkos92 - edit</t>
+  </si>
+  <si>
+    <t>PKMNTrainerRick - edit</t>
+  </si>
+  <si>
+    <t>done pokets3</t>
+  </si>
+  <si>
+    <t>yes ESY</t>
+  </si>
+  <si>
+    <t>PKMNTrainerRick_optimized</t>
+  </si>
+  <si>
+    <t>esy</t>
+  </si>
+  <si>
+    <t>pkmntrainerrick</t>
+  </si>
+  <si>
+    <t>bw3g</t>
+  </si>
+  <si>
+    <t>esy adapt</t>
+  </si>
+  <si>
+    <t>PKMNtrainerrick</t>
   </si>
 </sst>
 </file>
@@ -2858,7 +2897,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2881,6 +2920,7 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -12313,17 +12353,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{037CB756-8A09-4E44-9A4C-654D0B919B16}">
   <dimension ref="A2:K505"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A212" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D258" sqref="D258"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A213" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E264" sqref="E264"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="20.54296875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.453125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.90625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.26953125" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="10" bestFit="1" customWidth="1"/>
@@ -14576,8 +14616,24 @@
       <c r="B88" s="7" t="s">
         <v>241</v>
       </c>
-      <c r="D88" s="4"/>
-      <c r="F88" s="3"/>
+      <c r="C88" t="s">
+        <v>886</v>
+      </c>
+      <c r="D88" s="4" t="s">
+        <v>910</v>
+      </c>
+      <c r="E88" t="s">
+        <v>885</v>
+      </c>
+      <c r="F88" s="3" t="s">
+        <v>885</v>
+      </c>
+      <c r="G88" t="s">
+        <v>885</v>
+      </c>
+      <c r="H88" t="s">
+        <v>885</v>
+      </c>
     </row>
     <row r="89" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A89" s="1">
@@ -14586,8 +14642,24 @@
       <c r="B89" s="7" t="s">
         <v>237</v>
       </c>
-      <c r="D89" s="4"/>
-      <c r="F89" s="3"/>
+      <c r="C89" t="s">
+        <v>892</v>
+      </c>
+      <c r="D89" s="4" t="s">
+        <v>892</v>
+      </c>
+      <c r="E89" t="s">
+        <v>885</v>
+      </c>
+      <c r="F89" s="3" t="s">
+        <v>885</v>
+      </c>
+      <c r="G89" t="s">
+        <v>885</v>
+      </c>
+      <c r="H89" t="s">
+        <v>885</v>
+      </c>
     </row>
     <row r="90" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A90" s="1">
@@ -14596,8 +14668,24 @@
       <c r="B90" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="D90" s="4"/>
-      <c r="F90" s="3"/>
+      <c r="C90" t="s">
+        <v>898</v>
+      </c>
+      <c r="D90" s="4" t="s">
+        <v>898</v>
+      </c>
+      <c r="E90" t="s">
+        <v>885</v>
+      </c>
+      <c r="F90" s="3" t="s">
+        <v>885</v>
+      </c>
+      <c r="G90" t="s">
+        <v>885</v>
+      </c>
+      <c r="H90" t="s">
+        <v>885</v>
+      </c>
     </row>
     <row r="91" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A91" s="1">
@@ -14632,8 +14720,24 @@
       <c r="B92" s="7" t="s">
         <v>247</v>
       </c>
-      <c r="D92" s="4"/>
-      <c r="F92" s="3"/>
+      <c r="C92" t="s">
+        <v>911</v>
+      </c>
+      <c r="D92" s="4" t="s">
+        <v>912</v>
+      </c>
+      <c r="E92" t="s">
+        <v>885</v>
+      </c>
+      <c r="F92" s="3" t="s">
+        <v>885</v>
+      </c>
+      <c r="G92" t="s">
+        <v>885</v>
+      </c>
+      <c r="H92" t="s">
+        <v>885</v>
+      </c>
     </row>
     <row r="93" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A93" s="1">
@@ -14642,8 +14746,24 @@
       <c r="B93" s="7" t="s">
         <v>215</v>
       </c>
-      <c r="D93" s="4"/>
-      <c r="F93" s="3"/>
+      <c r="C93" t="s">
+        <v>914</v>
+      </c>
+      <c r="D93" s="4" t="s">
+        <v>914</v>
+      </c>
+      <c r="E93" t="s">
+        <v>873</v>
+      </c>
+      <c r="F93" s="3" t="s">
+        <v>873</v>
+      </c>
+      <c r="G93" t="s">
+        <v>873</v>
+      </c>
+      <c r="H93" t="s">
+        <v>873</v>
+      </c>
     </row>
     <row r="94" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A94" s="1">
@@ -14834,8 +14954,24 @@
       <c r="B101" s="7" t="s">
         <v>242</v>
       </c>
-      <c r="D101" s="4"/>
-      <c r="F101" s="3"/>
+      <c r="C101" t="s">
+        <v>913</v>
+      </c>
+      <c r="D101" s="4" t="s">
+        <v>915</v>
+      </c>
+      <c r="E101" t="s">
+        <v>885</v>
+      </c>
+      <c r="F101" s="3" t="s">
+        <v>885</v>
+      </c>
+      <c r="G101" t="s">
+        <v>885</v>
+      </c>
+      <c r="H101" t="s">
+        <v>885</v>
+      </c>
     </row>
     <row r="102" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A102" s="1">
@@ -14844,8 +14980,24 @@
       <c r="B102" s="7" t="s">
         <v>248</v>
       </c>
-      <c r="D102" s="4"/>
-      <c r="F102" s="3"/>
+      <c r="C102" t="s">
+        <v>885</v>
+      </c>
+      <c r="D102" s="4" t="s">
+        <v>915</v>
+      </c>
+      <c r="E102" t="s">
+        <v>885</v>
+      </c>
+      <c r="F102" s="3" t="s">
+        <v>885</v>
+      </c>
+      <c r="G102" t="s">
+        <v>885</v>
+      </c>
+      <c r="H102" t="s">
+        <v>885</v>
+      </c>
     </row>
     <row r="103" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A103">
@@ -14854,8 +15006,24 @@
       <c r="B103" s="7" t="s">
         <v>251</v>
       </c>
-      <c r="D103" s="4"/>
-      <c r="F103" s="3"/>
+      <c r="C103" t="s">
+        <v>886</v>
+      </c>
+      <c r="D103" s="4" t="s">
+        <v>905</v>
+      </c>
+      <c r="E103" t="s">
+        <v>885</v>
+      </c>
+      <c r="F103" s="3" t="s">
+        <v>885</v>
+      </c>
+      <c r="G103" t="s">
+        <v>885</v>
+      </c>
+      <c r="H103" t="s">
+        <v>885</v>
+      </c>
     </row>
     <row r="104" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A104">
@@ -14864,8 +15032,24 @@
       <c r="B104" s="7" t="s">
         <v>246</v>
       </c>
-      <c r="D104" s="4"/>
-      <c r="F104" s="3"/>
+      <c r="C104" t="s">
+        <v>885</v>
+      </c>
+      <c r="D104" s="4" t="s">
+        <v>905</v>
+      </c>
+      <c r="E104" t="s">
+        <v>885</v>
+      </c>
+      <c r="F104" s="3" t="s">
+        <v>885</v>
+      </c>
+      <c r="G104" t="s">
+        <v>885</v>
+      </c>
+      <c r="H104" t="s">
+        <v>885</v>
+      </c>
     </row>
     <row r="105" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A105">
@@ -14874,8 +15058,24 @@
       <c r="B105" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="D105" s="4"/>
-      <c r="F105" s="3"/>
+      <c r="C105" t="s">
+        <v>916</v>
+      </c>
+      <c r="D105" s="4" t="s">
+        <v>916</v>
+      </c>
+      <c r="E105" t="s">
+        <v>885</v>
+      </c>
+      <c r="F105" s="3" t="s">
+        <v>885</v>
+      </c>
+      <c r="G105" t="s">
+        <v>885</v>
+      </c>
+      <c r="H105" t="s">
+        <v>885</v>
+      </c>
     </row>
     <row r="106" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A106" s="1">
@@ -14936,8 +15136,24 @@
       <c r="B108" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="D108" s="4"/>
-      <c r="F108" s="3"/>
+      <c r="C108" t="s">
+        <v>885</v>
+      </c>
+      <c r="D108" s="4" t="s">
+        <v>885</v>
+      </c>
+      <c r="E108" t="s">
+        <v>885</v>
+      </c>
+      <c r="F108" s="3" t="s">
+        <v>885</v>
+      </c>
+      <c r="G108" t="s">
+        <v>885</v>
+      </c>
+      <c r="H108" t="s">
+        <v>885</v>
+      </c>
     </row>
     <row r="109" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A109">
@@ -15076,8 +15292,24 @@
       <c r="B114" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="D114" s="4"/>
-      <c r="F114" s="3"/>
+      <c r="C114" t="s">
+        <v>909</v>
+      </c>
+      <c r="D114" s="4" t="s">
+        <v>917</v>
+      </c>
+      <c r="E114" t="s">
+        <v>885</v>
+      </c>
+      <c r="F114" s="3" t="s">
+        <v>885</v>
+      </c>
+      <c r="G114" t="s">
+        <v>885</v>
+      </c>
+      <c r="H114" t="s">
+        <v>885</v>
+      </c>
     </row>
     <row r="115" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A115">
@@ -15242,8 +15474,24 @@
       <c r="B121" s="7" t="s">
         <v>214</v>
       </c>
-      <c r="D121" s="4"/>
-      <c r="F121" s="3"/>
+      <c r="C121" t="s">
+        <v>918</v>
+      </c>
+      <c r="D121" s="4" t="s">
+        <v>918</v>
+      </c>
+      <c r="E121" t="s">
+        <v>885</v>
+      </c>
+      <c r="F121" s="3" t="s">
+        <v>885</v>
+      </c>
+      <c r="G121" t="s">
+        <v>885</v>
+      </c>
+      <c r="H121" t="s">
+        <v>885</v>
+      </c>
     </row>
     <row r="122" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A122" s="1">
@@ -15278,8 +15526,24 @@
       <c r="B123" s="7" t="s">
         <v>198</v>
       </c>
-      <c r="D123" s="4"/>
-      <c r="F123" s="3"/>
+      <c r="C123" t="s">
+        <v>916</v>
+      </c>
+      <c r="D123" s="4" t="s">
+        <v>916</v>
+      </c>
+      <c r="E123" t="s">
+        <v>885</v>
+      </c>
+      <c r="F123" s="3" t="s">
+        <v>885</v>
+      </c>
+      <c r="G123" t="s">
+        <v>885</v>
+      </c>
+      <c r="H123" t="s">
+        <v>885</v>
+      </c>
     </row>
     <row r="124" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A124">
@@ -15288,8 +15552,24 @@
       <c r="B124" s="7" t="s">
         <v>199</v>
       </c>
-      <c r="D124" s="4"/>
-      <c r="F124" s="3"/>
+      <c r="C124" t="s">
+        <v>892</v>
+      </c>
+      <c r="D124" s="4" t="s">
+        <v>916</v>
+      </c>
+      <c r="E124" t="s">
+        <v>885</v>
+      </c>
+      <c r="F124" s="3" t="s">
+        <v>885</v>
+      </c>
+      <c r="G124" t="s">
+        <v>885</v>
+      </c>
+      <c r="H124" t="s">
+        <v>885</v>
+      </c>
     </row>
     <row r="125" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A125" s="1">
@@ -15818,8 +16098,24 @@
       <c r="B145" s="7" t="s">
         <v>192</v>
       </c>
-      <c r="D145" s="4"/>
-      <c r="F145" s="3"/>
+      <c r="C145" t="s">
+        <v>916</v>
+      </c>
+      <c r="D145" s="4" t="s">
+        <v>916</v>
+      </c>
+      <c r="E145" t="s">
+        <v>885</v>
+      </c>
+      <c r="F145" s="3" t="s">
+        <v>885</v>
+      </c>
+      <c r="G145" t="s">
+        <v>885</v>
+      </c>
+      <c r="H145" t="s">
+        <v>885</v>
+      </c>
     </row>
     <row r="146" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A146" s="1">
@@ -16114,8 +16410,24 @@
       <c r="B157" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D157" s="4"/>
-      <c r="F157" s="3"/>
+      <c r="C157" t="s">
+        <v>918</v>
+      </c>
+      <c r="D157" t="s">
+        <v>918</v>
+      </c>
+      <c r="E157" t="s">
+        <v>885</v>
+      </c>
+      <c r="F157" s="3" t="s">
+        <v>885</v>
+      </c>
+      <c r="G157" t="s">
+        <v>885</v>
+      </c>
+      <c r="H157" t="s">
+        <v>885</v>
+      </c>
     </row>
     <row r="158" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A158" s="1">
@@ -16124,8 +16436,24 @@
       <c r="B158" s="7" t="s">
         <v>168</v>
       </c>
-      <c r="D158" s="4"/>
-      <c r="F158" s="3"/>
+      <c r="C158" t="s">
+        <v>886</v>
+      </c>
+      <c r="D158" s="4" t="s">
+        <v>920</v>
+      </c>
+      <c r="E158" t="s">
+        <v>885</v>
+      </c>
+      <c r="F158" s="3" t="s">
+        <v>885</v>
+      </c>
+      <c r="G158" t="s">
+        <v>885</v>
+      </c>
+      <c r="H158" t="s">
+        <v>885</v>
+      </c>
     </row>
     <row r="159" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A159" s="1">
@@ -16628,8 +16956,24 @@
       <c r="B178" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="D178" s="4"/>
-      <c r="F178" s="3"/>
+      <c r="C178" t="s">
+        <v>916</v>
+      </c>
+      <c r="D178" s="4" t="s">
+        <v>916</v>
+      </c>
+      <c r="E178" t="s">
+        <v>885</v>
+      </c>
+      <c r="F178" s="3" t="s">
+        <v>885</v>
+      </c>
+      <c r="G178" t="s">
+        <v>885</v>
+      </c>
+      <c r="H178" t="s">
+        <v>885</v>
+      </c>
     </row>
     <row r="179" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A179" s="1">
@@ -16794,8 +17138,24 @@
       <c r="B185" s="7" t="s">
         <v>202</v>
       </c>
-      <c r="D185" s="4"/>
-      <c r="F185" s="3"/>
+      <c r="C185" t="s">
+        <v>919</v>
+      </c>
+      <c r="D185" s="4" t="s">
+        <v>919</v>
+      </c>
+      <c r="E185" t="s">
+        <v>885</v>
+      </c>
+      <c r="F185" s="3" t="s">
+        <v>885</v>
+      </c>
+      <c r="G185" t="s">
+        <v>885</v>
+      </c>
+      <c r="H185" t="s">
+        <v>885</v>
+      </c>
     </row>
     <row r="186" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A186" s="1">
@@ -16944,6 +17304,9 @@
       <c r="B192" s="7" t="s">
         <v>223</v>
       </c>
+      <c r="C192" t="s">
+        <v>884</v>
+      </c>
       <c r="D192" s="4"/>
       <c r="F192" s="3"/>
     </row>
@@ -17886,8 +18249,24 @@
       <c r="B235" s="7" t="s">
         <v>176</v>
       </c>
-      <c r="D235" s="4"/>
-      <c r="F235" s="3"/>
+      <c r="C235" t="s">
+        <v>909</v>
+      </c>
+      <c r="D235" s="4" t="s">
+        <v>905</v>
+      </c>
+      <c r="E235" t="s">
+        <v>885</v>
+      </c>
+      <c r="F235" s="3" t="s">
+        <v>885</v>
+      </c>
+      <c r="G235" t="s">
+        <v>885</v>
+      </c>
+      <c r="H235" t="s">
+        <v>885</v>
+      </c>
     </row>
     <row r="236" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A236">
@@ -18000,8 +18379,24 @@
       <c r="B240" s="7" t="s">
         <v>204</v>
       </c>
-      <c r="D240" s="4"/>
-      <c r="F240" s="3"/>
+      <c r="C240" t="s">
+        <v>892</v>
+      </c>
+      <c r="D240" s="4" t="s">
+        <v>908</v>
+      </c>
+      <c r="E240" t="s">
+        <v>885</v>
+      </c>
+      <c r="F240" s="3" t="s">
+        <v>885</v>
+      </c>
+      <c r="G240" t="s">
+        <v>885</v>
+      </c>
+      <c r="H240" t="s">
+        <v>885</v>
+      </c>
     </row>
     <row r="241" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A241" s="1">
@@ -18372,7 +18767,7 @@
       <c r="B255" s="3"/>
       <c r="C255" s="10">
         <f>COUNTA(C4:D254)-(2*COUNTA(B4:B254))</f>
-        <v>-68</v>
+        <v>-23</v>
       </c>
     </row>
     <row r="256" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
@@ -18398,26 +18793,62 @@
     <row r="258" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A258" s="1"/>
       <c r="B258" s="3"/>
+      <c r="D258" s="11">
+        <v>45267</v>
+      </c>
+      <c r="E258">
+        <v>64</v>
+      </c>
     </row>
     <row r="259" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A259" s="1"/>
       <c r="B259" s="3"/>
+      <c r="D259" s="11">
+        <v>45268</v>
+      </c>
+      <c r="E259">
+        <v>60</v>
+      </c>
     </row>
     <row r="260" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A260" s="1"/>
       <c r="B260" s="3"/>
+      <c r="D260" s="11">
+        <v>45271</v>
+      </c>
+      <c r="E260">
+        <v>52</v>
+      </c>
     </row>
     <row r="261" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A261" s="1"/>
       <c r="B261" s="3"/>
+      <c r="D261" s="12">
+        <v>45272</v>
+      </c>
+      <c r="E261">
+        <v>48</v>
+      </c>
     </row>
     <row r="262" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A262" s="1"/>
       <c r="B262" s="3"/>
+      <c r="D262" s="12">
+        <v>45273</v>
+      </c>
+      <c r="E262">
+        <v>46</v>
+      </c>
     </row>
     <row r="263" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A263" s="1"/>
       <c r="B263" s="3"/>
+      <c r="D263" s="12">
+        <v>45274</v>
+      </c>
+      <c r="E263">
+        <v>23</v>
+      </c>
     </row>
     <row r="264" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A264" s="1"/>

</xml_diff>